<commit_message>
implemented unviable routes code
</commit_message>
<xml_diff>
--- a/VRPTW-New/Zeus OS VRPTW Workspace 2018 2.4/Zeus/data/VRPTW/Results/R201_I1_LongResults.xlsx
+++ b/VRPTW-New/Zeus OS VRPTW Workspace 2018 2.4/Zeus/data/VRPTW/Results/R201_I1_LongResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2944" uniqueCount="25">
   <si>
     <t/>
   </si>
@@ -94,13 +94,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -133,10 +143,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -159,26 +171,26 @@
     <col min="8" max="8" bestFit="true" customWidth="true" width="14.71875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true">
-      <c r="A1" t="s" s="2">
+    <row r="1" s="4" customFormat="true">
+      <c r="A1" t="s" s="4">
         <v>1</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" t="s" s="4">
         <v>4</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" t="s" s="4">
         <v>7</v>
       </c>
     </row>
@@ -206,28 +218,28 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="2">
+      <c r="A3" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B3" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C3" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s" s="2">
+      <c r="C3" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E3" t="s" s="2">
+      <c r="E3" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F3" t="s" s="2">
+      <c r="F3" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G3" t="s" s="2">
+      <c r="G3" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H3" t="s" s="2">
+      <c r="H3" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -252,28 +264,28 @@
       </c>
     </row>
     <row r="5">
-      <c r="B5" t="s" s="2">
+      <c r="B5" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C5" t="s" s="2">
+      <c r="C5" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D5" t="s" s="2">
+      <c r="D5" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E5" t="s" s="2">
+      <c r="E5" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F5" t="s" s="2">
+      <c r="F5" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G5" t="s" s="2">
+      <c r="G5" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H5" t="s" s="2">
+      <c r="H5" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I5" t="s" s="2">
+      <c r="I5" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -448,10 +460,10 @@
       <c r="I11">
         <f>((C11-C10)^2+(D11- D10)^2)^.5</f>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="2" t="s">
+      <c r="J11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L11" t="n">
@@ -495,28 +507,28 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="2">
+      <c r="A13" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B13" t="s" s="2">
+      <c r="B13" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C13" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s" s="2">
+      <c r="C13" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E13" t="s" s="2">
+      <c r="E13" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F13" t="s" s="2">
+      <c r="F13" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G13" t="s" s="2">
+      <c r="G13" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H13" t="s" s="2">
+      <c r="H13" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -541,28 +553,28 @@
       </c>
     </row>
     <row r="15">
-      <c r="B15" t="s" s="2">
+      <c r="B15" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C15" t="s" s="2">
+      <c r="C15" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D15" t="s" s="2">
+      <c r="D15" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E15" t="s" s="2">
+      <c r="E15" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F15" t="s" s="2">
+      <c r="F15" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G15" t="s" s="2">
+      <c r="G15" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H15" t="s" s="2">
+      <c r="H15" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I15" t="s" s="2">
+      <c r="I15" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -650,10 +662,10 @@
       <c r="I18">
         <f>((C18-C17)^2+(D18- D17)^2)^.5</f>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="2" t="s">
+      <c r="J18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L18" t="n">
@@ -697,28 +709,28 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s" s="2">
+      <c r="A20" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B20" t="s" s="2">
+      <c r="B20" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C20" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D20" t="s" s="2">
+      <c r="C20" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E20" t="s" s="2">
+      <c r="E20" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F20" t="s" s="2">
+      <c r="F20" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G20" t="s" s="2">
+      <c r="G20" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H20" t="s" s="2">
+      <c r="H20" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -743,28 +755,28 @@
       </c>
     </row>
     <row r="22">
-      <c r="B22" t="s" s="2">
+      <c r="B22" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C22" t="s" s="2">
+      <c r="C22" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D22" t="s" s="2">
+      <c r="D22" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E22" t="s" s="2">
+      <c r="E22" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F22" t="s" s="2">
+      <c r="F22" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G22" t="s" s="2">
+      <c r="G22" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H22" t="s" s="2">
+      <c r="H22" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I22" t="s" s="2">
+      <c r="I22" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -881,10 +893,10 @@
       <c r="I26">
         <f>((C26-C25)^2+(D26- D25)^2)^.5</f>
       </c>
-      <c r="J26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K26" s="2" t="s">
+      <c r="J26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L26" t="n">
@@ -928,28 +940,28 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s" s="2">
+      <c r="A28" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B28" t="s" s="2">
+      <c r="B28" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C28" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D28" t="s" s="2">
+      <c r="C28" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E28" t="s" s="2">
+      <c r="E28" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F28" t="s" s="2">
+      <c r="F28" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G28" t="s" s="2">
+      <c r="G28" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H28" t="s" s="2">
+      <c r="H28" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -974,28 +986,28 @@
       </c>
     </row>
     <row r="30">
-      <c r="B30" t="s" s="2">
+      <c r="B30" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C30" t="s" s="2">
+      <c r="C30" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D30" t="s" s="2">
+      <c r="D30" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E30" t="s" s="2">
+      <c r="E30" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F30" t="s" s="2">
+      <c r="F30" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G30" t="s" s="2">
+      <c r="G30" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H30" t="s" s="2">
+      <c r="H30" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I30" t="s" s="2">
+      <c r="I30" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -1112,10 +1124,10 @@
       <c r="I34">
         <f>((C34-C33)^2+(D34- D33)^2)^.5</f>
       </c>
-      <c r="J34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K34" s="2" t="s">
+      <c r="J34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L34" t="n">
@@ -1159,28 +1171,28 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s" s="2">
+      <c r="A36" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B36" t="s" s="2">
+      <c r="B36" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C36" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D36" t="s" s="2">
+      <c r="C36" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E36" t="s" s="2">
+      <c r="E36" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F36" t="s" s="2">
+      <c r="F36" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G36" t="s" s="2">
+      <c r="G36" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H36" t="s" s="2">
+      <c r="H36" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -1205,28 +1217,28 @@
       </c>
     </row>
     <row r="38">
-      <c r="B38" t="s" s="2">
+      <c r="B38" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C38" t="s" s="2">
+      <c r="C38" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D38" t="s" s="2">
+      <c r="D38" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E38" t="s" s="2">
+      <c r="E38" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F38" t="s" s="2">
+      <c r="F38" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G38" t="s" s="2">
+      <c r="G38" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H38" t="s" s="2">
+      <c r="H38" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I38" t="s" s="2">
+      <c r="I38" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -1401,10 +1413,10 @@
       <c r="I44">
         <f>((C44-C43)^2+(D44- D43)^2)^.5</f>
       </c>
-      <c r="J44" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K44" s="2" t="s">
+      <c r="J44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K44" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L44" t="n">
@@ -1448,28 +1460,28 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="s" s="2">
+      <c r="A46" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B46" t="s" s="2">
+      <c r="B46" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C46" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D46" t="s" s="2">
+      <c r="C46" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D46" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E46" t="s" s="2">
+      <c r="E46" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F46" t="s" s="2">
+      <c r="F46" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G46" t="s" s="2">
+      <c r="G46" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H46" t="s" s="2">
+      <c r="H46" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -1494,28 +1506,28 @@
       </c>
     </row>
     <row r="48">
-      <c r="B48" t="s" s="2">
+      <c r="B48" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C48" t="s" s="2">
+      <c r="C48" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D48" t="s" s="2">
+      <c r="D48" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E48" t="s" s="2">
+      <c r="E48" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F48" t="s" s="2">
+      <c r="F48" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G48" t="s" s="2">
+      <c r="G48" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H48" t="s" s="2">
+      <c r="H48" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I48" t="s" s="2">
+      <c r="I48" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -1632,10 +1644,10 @@
       <c r="I52">
         <f>((C52-C51)^2+(D52- D51)^2)^.5</f>
       </c>
-      <c r="J52" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K52" s="2" t="s">
+      <c r="J52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K52" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L52" t="n">
@@ -1679,28 +1691,28 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="s" s="2">
+      <c r="A54" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B54" t="s" s="2">
+      <c r="B54" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C54" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D54" t="s" s="2">
+      <c r="C54" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D54" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E54" t="s" s="2">
+      <c r="E54" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F54" t="s" s="2">
+      <c r="F54" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G54" t="s" s="2">
+      <c r="G54" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H54" t="s" s="2">
+      <c r="H54" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -1725,28 +1737,28 @@
       </c>
     </row>
     <row r="56">
-      <c r="B56" t="s" s="2">
+      <c r="B56" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C56" t="s" s="2">
+      <c r="C56" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D56" t="s" s="2">
+      <c r="D56" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E56" t="s" s="2">
+      <c r="E56" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F56" t="s" s="2">
+      <c r="F56" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G56" t="s" s="2">
+      <c r="G56" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H56" t="s" s="2">
+      <c r="H56" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I56" t="s" s="2">
+      <c r="I56" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -1892,10 +1904,10 @@
       <c r="I61">
         <f>((C61-C60)^2+(D61- D60)^2)^.5</f>
       </c>
-      <c r="J61" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K61" s="2" t="s">
+      <c r="J61" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K61" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L61" t="n">
@@ -1939,28 +1951,28 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="s" s="2">
+      <c r="A63" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B63" t="s" s="2">
+      <c r="B63" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C63" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D63" t="s" s="2">
+      <c r="C63" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D63" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E63" t="s" s="2">
+      <c r="E63" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F63" t="s" s="2">
+      <c r="F63" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G63" t="s" s="2">
+      <c r="G63" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H63" t="s" s="2">
+      <c r="H63" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -1985,28 +1997,28 @@
       </c>
     </row>
     <row r="65">
-      <c r="B65" t="s" s="2">
+      <c r="B65" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C65" t="s" s="2">
+      <c r="C65" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D65" t="s" s="2">
+      <c r="D65" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E65" t="s" s="2">
+      <c r="E65" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F65" t="s" s="2">
+      <c r="F65" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G65" t="s" s="2">
+      <c r="G65" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H65" t="s" s="2">
+      <c r="H65" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I65" t="s" s="2">
+      <c r="I65" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -2094,10 +2106,10 @@
       <c r="I68">
         <f>((C68-C67)^2+(D68- D67)^2)^.5</f>
       </c>
-      <c r="J68" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K68" s="2" t="s">
+      <c r="J68" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K68" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L68" t="n">
@@ -2141,28 +2153,28 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="s" s="2">
+      <c r="A70" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B70" t="s" s="2">
+      <c r="B70" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C70" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D70" t="s" s="2">
+      <c r="C70" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D70" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E70" t="s" s="2">
+      <c r="E70" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F70" t="s" s="2">
+      <c r="F70" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G70" t="s" s="2">
+      <c r="G70" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H70" t="s" s="2">
+      <c r="H70" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -2187,28 +2199,28 @@
       </c>
     </row>
     <row r="72">
-      <c r="B72" t="s" s="2">
+      <c r="B72" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C72" t="s" s="2">
+      <c r="C72" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D72" t="s" s="2">
+      <c r="D72" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E72" t="s" s="2">
+      <c r="E72" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F72" t="s" s="2">
+      <c r="F72" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G72" t="s" s="2">
+      <c r="G72" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H72" t="s" s="2">
+      <c r="H72" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I72" t="s" s="2">
+      <c r="I72" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -2325,10 +2337,10 @@
       <c r="I76">
         <f>((C76-C75)^2+(D76- D75)^2)^.5</f>
       </c>
-      <c r="J76" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K76" s="2" t="s">
+      <c r="J76" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K76" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L76" t="n">
@@ -2372,28 +2384,28 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="s" s="2">
+      <c r="A78" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B78" t="s" s="2">
+      <c r="B78" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C78" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D78" t="s" s="2">
+      <c r="C78" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D78" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E78" t="s" s="2">
+      <c r="E78" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F78" t="s" s="2">
+      <c r="F78" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G78" t="s" s="2">
+      <c r="G78" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H78" t="s" s="2">
+      <c r="H78" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -2418,28 +2430,28 @@
       </c>
     </row>
     <row r="80">
-      <c r="B80" t="s" s="2">
+      <c r="B80" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C80" t="s" s="2">
+      <c r="C80" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D80" t="s" s="2">
+      <c r="D80" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E80" t="s" s="2">
+      <c r="E80" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F80" t="s" s="2">
+      <c r="F80" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G80" t="s" s="2">
+      <c r="G80" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H80" t="s" s="2">
+      <c r="H80" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I80" t="s" s="2">
+      <c r="I80" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -2556,10 +2568,10 @@
       <c r="I84">
         <f>((C84-C83)^2+(D84- D83)^2)^.5</f>
       </c>
-      <c r="J84" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K84" s="2" t="s">
+      <c r="J84" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K84" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L84" t="n">
@@ -2603,28 +2615,28 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="s" s="2">
+      <c r="A86" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B86" t="s" s="2">
+      <c r="B86" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C86" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D86" t="s" s="2">
+      <c r="C86" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D86" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E86" t="s" s="2">
+      <c r="E86" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F86" t="s" s="2">
+      <c r="F86" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G86" t="s" s="2">
+      <c r="G86" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H86" t="s" s="2">
+      <c r="H86" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -2649,28 +2661,28 @@
       </c>
     </row>
     <row r="88">
-      <c r="B88" t="s" s="2">
+      <c r="B88" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C88" t="s" s="2">
+      <c r="C88" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D88" t="s" s="2">
+      <c r="D88" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E88" t="s" s="2">
+      <c r="E88" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F88" t="s" s="2">
+      <c r="F88" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G88" t="s" s="2">
+      <c r="G88" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H88" t="s" s="2">
+      <c r="H88" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I88" t="s" s="2">
+      <c r="I88" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -2758,10 +2770,10 @@
       <c r="I91">
         <f>((C91-C90)^2+(D91- D90)^2)^.5</f>
       </c>
-      <c r="J91" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K91" s="2" t="s">
+      <c r="J91" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K91" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L91" t="n">
@@ -2805,28 +2817,28 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="s" s="2">
+      <c r="A93" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B93" t="s" s="2">
+      <c r="B93" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C93" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D93" t="s" s="2">
+      <c r="C93" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D93" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E93" t="s" s="2">
+      <c r="E93" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F93" t="s" s="2">
+      <c r="F93" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G93" t="s" s="2">
+      <c r="G93" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H93" t="s" s="2">
+      <c r="H93" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -2851,28 +2863,28 @@
       </c>
     </row>
     <row r="95">
-      <c r="B95" t="s" s="2">
+      <c r="B95" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C95" t="s" s="2">
+      <c r="C95" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D95" t="s" s="2">
+      <c r="D95" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E95" t="s" s="2">
+      <c r="E95" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F95" t="s" s="2">
+      <c r="F95" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G95" t="s" s="2">
+      <c r="G95" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H95" t="s" s="2">
+      <c r="H95" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I95" t="s" s="2">
+      <c r="I95" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -2960,10 +2972,10 @@
       <c r="I98">
         <f>((C98-C97)^2+(D98- D97)^2)^.5</f>
       </c>
-      <c r="J98" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K98" s="2" t="s">
+      <c r="J98" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K98" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L98" t="n">
@@ -3007,28 +3019,28 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="s" s="2">
+      <c r="A100" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B100" t="s" s="2">
+      <c r="B100" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C100" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D100" t="s" s="2">
+      <c r="C100" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D100" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E100" t="s" s="2">
+      <c r="E100" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F100" t="s" s="2">
+      <c r="F100" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G100" t="s" s="2">
+      <c r="G100" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H100" t="s" s="2">
+      <c r="H100" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -3053,28 +3065,28 @@
       </c>
     </row>
     <row r="102">
-      <c r="B102" t="s" s="2">
+      <c r="B102" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C102" t="s" s="2">
+      <c r="C102" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D102" t="s" s="2">
+      <c r="D102" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E102" t="s" s="2">
+      <c r="E102" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F102" t="s" s="2">
+      <c r="F102" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G102" t="s" s="2">
+      <c r="G102" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H102" t="s" s="2">
+      <c r="H102" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I102" t="s" s="2">
+      <c r="I102" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -3220,10 +3232,10 @@
       <c r="I107">
         <f>((C107-C106)^2+(D107- D106)^2)^.5</f>
       </c>
-      <c r="J107" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K107" s="2" t="s">
+      <c r="J107" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K107" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L107" t="n">
@@ -3267,28 +3279,28 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="s" s="2">
+      <c r="A109" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B109" t="s" s="2">
+      <c r="B109" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C109" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D109" t="s" s="2">
+      <c r="C109" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D109" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E109" t="s" s="2">
+      <c r="E109" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F109" t="s" s="2">
+      <c r="F109" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G109" t="s" s="2">
+      <c r="G109" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H109" t="s" s="2">
+      <c r="H109" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -3313,28 +3325,28 @@
       </c>
     </row>
     <row r="111">
-      <c r="B111" t="s" s="2">
+      <c r="B111" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C111" t="s" s="2">
+      <c r="C111" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D111" t="s" s="2">
+      <c r="D111" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E111" t="s" s="2">
+      <c r="E111" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F111" t="s" s="2">
+      <c r="F111" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G111" t="s" s="2">
+      <c r="G111" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H111" t="s" s="2">
+      <c r="H111" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I111" t="s" s="2">
+      <c r="I111" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -3393,10 +3405,10 @@
       <c r="I113">
         <f>((C113-C112)^2+(D113- D112)^2)^.5</f>
       </c>
-      <c r="J113" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K113" s="2" t="s">
+      <c r="J113" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K113" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L113" t="n">
@@ -3440,28 +3452,28 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="s" s="2">
+      <c r="A115" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B115" t="s" s="2">
+      <c r="B115" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C115" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D115" t="s" s="2">
+      <c r="C115" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D115" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E115" t="s" s="2">
+      <c r="E115" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F115" t="s" s="2">
+      <c r="F115" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G115" t="s" s="2">
+      <c r="G115" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H115" t="s" s="2">
+      <c r="H115" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -3486,28 +3498,28 @@
       </c>
     </row>
     <row r="117">
-      <c r="B117" t="s" s="2">
+      <c r="B117" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C117" t="s" s="2">
+      <c r="C117" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D117" t="s" s="2">
+      <c r="D117" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E117" t="s" s="2">
+      <c r="E117" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F117" t="s" s="2">
+      <c r="F117" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G117" t="s" s="2">
+      <c r="G117" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H117" t="s" s="2">
+      <c r="H117" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I117" t="s" s="2">
+      <c r="I117" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -3595,10 +3607,10 @@
       <c r="I120">
         <f>((C120-C119)^2+(D120- D119)^2)^.5</f>
       </c>
-      <c r="J120" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K120" s="2" t="s">
+      <c r="J120" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K120" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L120" t="n">
@@ -3642,28 +3654,28 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="s" s="2">
+      <c r="A122" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B122" t="s" s="2">
+      <c r="B122" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C122" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D122" t="s" s="2">
+      <c r="C122" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D122" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E122" t="s" s="2">
+      <c r="E122" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F122" t="s" s="2">
+      <c r="F122" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G122" t="s" s="2">
+      <c r="G122" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H122" t="s" s="2">
+      <c r="H122" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -3688,28 +3700,28 @@
       </c>
     </row>
     <row r="124">
-      <c r="B124" t="s" s="2">
+      <c r="B124" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C124" t="s" s="2">
+      <c r="C124" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D124" t="s" s="2">
+      <c r="D124" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E124" t="s" s="2">
+      <c r="E124" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F124" t="s" s="2">
+      <c r="F124" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G124" t="s" s="2">
+      <c r="G124" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H124" t="s" s="2">
+      <c r="H124" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I124" t="s" s="2">
+      <c r="I124" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -3826,10 +3838,10 @@
       <c r="I128">
         <f>((C128-C127)^2+(D128- D127)^2)^.5</f>
       </c>
-      <c r="J128" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K128" s="2" t="s">
+      <c r="J128" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K128" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L128" t="n">
@@ -3873,28 +3885,28 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="s" s="2">
+      <c r="A130" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B130" t="s" s="2">
+      <c r="B130" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C130" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D130" t="s" s="2">
+      <c r="C130" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D130" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E130" t="s" s="2">
+      <c r="E130" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F130" t="s" s="2">
+      <c r="F130" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G130" t="s" s="2">
+      <c r="G130" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H130" t="s" s="2">
+      <c r="H130" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -3919,28 +3931,28 @@
       </c>
     </row>
     <row r="132">
-      <c r="B132" t="s" s="2">
+      <c r="B132" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C132" t="s" s="2">
+      <c r="C132" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D132" t="s" s="2">
+      <c r="D132" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E132" t="s" s="2">
+      <c r="E132" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F132" t="s" s="2">
+      <c r="F132" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G132" t="s" s="2">
+      <c r="G132" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H132" t="s" s="2">
+      <c r="H132" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I132" t="s" s="2">
+      <c r="I132" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -3999,10 +4011,10 @@
       <c r="I134">
         <f>((C134-C133)^2+(D134- D133)^2)^.5</f>
       </c>
-      <c r="J134" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K134" s="2" t="s">
+      <c r="J134" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K134" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L134" t="n">
@@ -4046,28 +4058,28 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" t="s" s="2">
+      <c r="A136" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B136" t="s" s="2">
+      <c r="B136" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C136" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D136" t="s" s="2">
+      <c r="C136" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D136" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E136" t="s" s="2">
+      <c r="E136" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F136" t="s" s="2">
+      <c r="F136" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G136" t="s" s="2">
+      <c r="G136" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H136" t="s" s="2">
+      <c r="H136" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -4092,28 +4104,28 @@
       </c>
     </row>
     <row r="138">
-      <c r="B138" t="s" s="2">
+      <c r="B138" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C138" t="s" s="2">
+      <c r="C138" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D138" t="s" s="2">
+      <c r="D138" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E138" t="s" s="2">
+      <c r="E138" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F138" t="s" s="2">
+      <c r="F138" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G138" t="s" s="2">
+      <c r="G138" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H138" t="s" s="2">
+      <c r="H138" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I138" t="s" s="2">
+      <c r="I138" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -4230,10 +4242,10 @@
       <c r="I142">
         <f>((C142-C141)^2+(D142- D141)^2)^.5</f>
       </c>
-      <c r="J142" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K142" s="2" t="s">
+      <c r="J142" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K142" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L142" t="n">
@@ -4277,28 +4289,28 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" t="s" s="2">
+      <c r="A144" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B144" t="s" s="2">
+      <c r="B144" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C144" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D144" t="s" s="2">
+      <c r="C144" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D144" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E144" t="s" s="2">
+      <c r="E144" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F144" t="s" s="2">
+      <c r="F144" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G144" t="s" s="2">
+      <c r="G144" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H144" t="s" s="2">
+      <c r="H144" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -4323,28 +4335,28 @@
       </c>
     </row>
     <row r="146">
-      <c r="B146" t="s" s="2">
+      <c r="B146" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C146" t="s" s="2">
+      <c r="C146" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D146" t="s" s="2">
+      <c r="D146" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E146" t="s" s="2">
+      <c r="E146" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F146" t="s" s="2">
+      <c r="F146" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G146" t="s" s="2">
+      <c r="G146" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H146" t="s" s="2">
+      <c r="H146" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I146" t="s" s="2">
+      <c r="I146" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -4461,10 +4473,10 @@
       <c r="I150">
         <f>((C150-C149)^2+(D150- D149)^2)^.5</f>
       </c>
-      <c r="J150" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K150" s="2" t="s">
+      <c r="J150" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K150" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L150" t="n">
@@ -4508,28 +4520,28 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" t="s" s="2">
+      <c r="A152" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B152" t="s" s="2">
+      <c r="B152" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C152" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D152" t="s" s="2">
+      <c r="C152" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D152" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E152" t="s" s="2">
+      <c r="E152" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F152" t="s" s="2">
+      <c r="F152" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G152" t="s" s="2">
+      <c r="G152" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H152" t="s" s="2">
+      <c r="H152" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -4554,28 +4566,28 @@
       </c>
     </row>
     <row r="154">
-      <c r="B154" t="s" s="2">
+      <c r="B154" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C154" t="s" s="2">
+      <c r="C154" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D154" t="s" s="2">
+      <c r="D154" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E154" t="s" s="2">
+      <c r="E154" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F154" t="s" s="2">
+      <c r="F154" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G154" t="s" s="2">
+      <c r="G154" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H154" t="s" s="2">
+      <c r="H154" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I154" t="s" s="2">
+      <c r="I154" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -4750,10 +4762,10 @@
       <c r="I160">
         <f>((C160-C159)^2+(D160- D159)^2)^.5</f>
       </c>
-      <c r="J160" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K160" s="2" t="s">
+      <c r="J160" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K160" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L160" t="n">
@@ -4797,28 +4809,28 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" t="s" s="2">
+      <c r="A162" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B162" t="s" s="2">
+      <c r="B162" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C162" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D162" t="s" s="2">
+      <c r="C162" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D162" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E162" t="s" s="2">
+      <c r="E162" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F162" t="s" s="2">
+      <c r="F162" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G162" t="s" s="2">
+      <c r="G162" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H162" t="s" s="2">
+      <c r="H162" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -4843,28 +4855,28 @@
       </c>
     </row>
     <row r="164">
-      <c r="B164" t="s" s="2">
+      <c r="B164" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C164" t="s" s="2">
+      <c r="C164" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D164" t="s" s="2">
+      <c r="D164" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E164" t="s" s="2">
+      <c r="E164" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F164" t="s" s="2">
+      <c r="F164" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G164" t="s" s="2">
+      <c r="G164" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H164" t="s" s="2">
+      <c r="H164" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I164" t="s" s="2">
+      <c r="I164" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -4923,10 +4935,10 @@
       <c r="I166">
         <f>((C166-C165)^2+(D166- D165)^2)^.5</f>
       </c>
-      <c r="J166" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K166" s="2" t="s">
+      <c r="J166" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K166" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L166" t="n">
@@ -4970,28 +4982,28 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="s" s="2">
+      <c r="A168" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B168" t="s" s="2">
+      <c r="B168" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C168" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D168" t="s" s="2">
+      <c r="C168" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D168" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E168" t="s" s="2">
+      <c r="E168" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F168" t="s" s="2">
+      <c r="F168" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G168" t="s" s="2">
+      <c r="G168" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H168" t="s" s="2">
+      <c r="H168" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -5016,28 +5028,28 @@
       </c>
     </row>
     <row r="170">
-      <c r="B170" t="s" s="2">
+      <c r="B170" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C170" t="s" s="2">
+      <c r="C170" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D170" t="s" s="2">
+      <c r="D170" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E170" t="s" s="2">
+      <c r="E170" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F170" t="s" s="2">
+      <c r="F170" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G170" t="s" s="2">
+      <c r="G170" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H170" t="s" s="2">
+      <c r="H170" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I170" t="s" s="2">
+      <c r="I170" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -5096,10 +5108,10 @@
       <c r="I172">
         <f>((C172-C171)^2+(D172- D171)^2)^.5</f>
       </c>
-      <c r="J172" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K172" s="2" t="s">
+      <c r="J172" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K172" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L172" t="n">
@@ -5143,28 +5155,28 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" t="s" s="2">
+      <c r="A174" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B174" t="s" s="2">
+      <c r="B174" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C174" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D174" t="s" s="2">
+      <c r="C174" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D174" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E174" t="s" s="2">
+      <c r="E174" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F174" t="s" s="2">
+      <c r="F174" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G174" t="s" s="2">
+      <c r="G174" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H174" t="s" s="2">
+      <c r="H174" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -5189,28 +5201,28 @@
       </c>
     </row>
     <row r="176">
-      <c r="B176" t="s" s="2">
+      <c r="B176" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C176" t="s" s="2">
+      <c r="C176" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D176" t="s" s="2">
+      <c r="D176" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E176" t="s" s="2">
+      <c r="E176" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F176" t="s" s="2">
+      <c r="F176" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G176" t="s" s="2">
+      <c r="G176" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H176" t="s" s="2">
+      <c r="H176" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I176" t="s" s="2">
+      <c r="I176" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -5298,10 +5310,10 @@
       <c r="I179">
         <f>((C179-C178)^2+(D179- D178)^2)^.5</f>
       </c>
-      <c r="J179" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K179" s="2" t="s">
+      <c r="J179" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K179" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L179" t="n">
@@ -5345,28 +5357,28 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" t="s" s="2">
+      <c r="A181" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B181" t="s" s="2">
+      <c r="B181" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C181" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D181" t="s" s="2">
+      <c r="C181" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D181" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E181" t="s" s="2">
+      <c r="E181" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F181" t="s" s="2">
+      <c r="F181" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G181" t="s" s="2">
+      <c r="G181" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H181" t="s" s="2">
+      <c r="H181" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -5391,28 +5403,28 @@
       </c>
     </row>
     <row r="183">
-      <c r="B183" t="s" s="2">
+      <c r="B183" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C183" t="s" s="2">
+      <c r="C183" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D183" t="s" s="2">
+      <c r="D183" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E183" t="s" s="2">
+      <c r="E183" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F183" t="s" s="2">
+      <c r="F183" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G183" t="s" s="2">
+      <c r="G183" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H183" t="s" s="2">
+      <c r="H183" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I183" t="s" s="2">
+      <c r="I183" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -5500,10 +5512,10 @@
       <c r="I186">
         <f>((C186-C185)^2+(D186- D185)^2)^.5</f>
       </c>
-      <c r="J186" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K186" s="2" t="s">
+      <c r="J186" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K186" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L186" t="n">
@@ -5547,28 +5559,28 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" t="s" s="2">
+      <c r="A188" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B188" t="s" s="2">
+      <c r="B188" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C188" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D188" t="s" s="2">
+      <c r="C188" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D188" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E188" t="s" s="2">
+      <c r="E188" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F188" t="s" s="2">
+      <c r="F188" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G188" t="s" s="2">
+      <c r="G188" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H188" t="s" s="2">
+      <c r="H188" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -5593,28 +5605,28 @@
       </c>
     </row>
     <row r="190">
-      <c r="B190" t="s" s="2">
+      <c r="B190" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C190" t="s" s="2">
+      <c r="C190" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D190" t="s" s="2">
+      <c r="D190" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E190" t="s" s="2">
+      <c r="E190" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F190" t="s" s="2">
+      <c r="F190" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G190" t="s" s="2">
+      <c r="G190" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H190" t="s" s="2">
+      <c r="H190" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I190" t="s" s="2">
+      <c r="I190" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -5760,10 +5772,10 @@
       <c r="I195">
         <f>((C195-C194)^2+(D195- D194)^2)^.5</f>
       </c>
-      <c r="J195" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K195" s="2" t="s">
+      <c r="J195" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K195" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L195" t="n">
@@ -5807,28 +5819,28 @@
       </c>
     </row>
     <row r="197">
-      <c r="A197" t="s" s="2">
+      <c r="A197" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B197" t="s" s="2">
+      <c r="B197" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C197" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D197" t="s" s="2">
+      <c r="C197" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D197" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E197" t="s" s="2">
+      <c r="E197" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F197" t="s" s="2">
+      <c r="F197" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G197" t="s" s="2">
+      <c r="G197" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H197" t="s" s="2">
+      <c r="H197" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -5853,28 +5865,28 @@
       </c>
     </row>
     <row r="199">
-      <c r="B199" t="s" s="2">
+      <c r="B199" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C199" t="s" s="2">
+      <c r="C199" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D199" t="s" s="2">
+      <c r="D199" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E199" t="s" s="2">
+      <c r="E199" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F199" t="s" s="2">
+      <c r="F199" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G199" t="s" s="2">
+      <c r="G199" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H199" t="s" s="2">
+      <c r="H199" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I199" t="s" s="2">
+      <c r="I199" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -5991,10 +6003,10 @@
       <c r="I203">
         <f>((C203-C202)^2+(D203- D202)^2)^.5</f>
       </c>
-      <c r="J203" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K203" s="2" t="s">
+      <c r="J203" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K203" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L203" t="n">
@@ -6038,28 +6050,28 @@
       </c>
     </row>
     <row r="205">
-      <c r="A205" t="s" s="2">
+      <c r="A205" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B205" t="s" s="2">
+      <c r="B205" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C205" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D205" t="s" s="2">
+      <c r="C205" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D205" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E205" t="s" s="2">
+      <c r="E205" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F205" t="s" s="2">
+      <c r="F205" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G205" t="s" s="2">
+      <c r="G205" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H205" t="s" s="2">
+      <c r="H205" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -6084,28 +6096,28 @@
       </c>
     </row>
     <row r="207">
-      <c r="B207" t="s" s="2">
+      <c r="B207" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C207" t="s" s="2">
+      <c r="C207" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D207" t="s" s="2">
+      <c r="D207" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E207" t="s" s="2">
+      <c r="E207" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F207" t="s" s="2">
+      <c r="F207" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G207" t="s" s="2">
+      <c r="G207" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H207" t="s" s="2">
+      <c r="H207" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I207" t="s" s="2">
+      <c r="I207" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -6164,10 +6176,10 @@
       <c r="I209">
         <f>((C209-C208)^2+(D209- D208)^2)^.5</f>
       </c>
-      <c r="J209" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K209" s="2" t="s">
+      <c r="J209" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K209" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L209" t="n">
@@ -6211,28 +6223,28 @@
       </c>
     </row>
     <row r="211">
-      <c r="A211" t="s" s="2">
+      <c r="A211" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B211" t="s" s="2">
+      <c r="B211" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C211" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D211" t="s" s="2">
+      <c r="C211" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D211" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E211" t="s" s="2">
+      <c r="E211" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F211" t="s" s="2">
+      <c r="F211" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G211" t="s" s="2">
+      <c r="G211" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H211" t="s" s="2">
+      <c r="H211" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -6257,28 +6269,28 @@
       </c>
     </row>
     <row r="213">
-      <c r="B213" t="s" s="2">
+      <c r="B213" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C213" t="s" s="2">
+      <c r="C213" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D213" t="s" s="2">
+      <c r="D213" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E213" t="s" s="2">
+      <c r="E213" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F213" t="s" s="2">
+      <c r="F213" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G213" t="s" s="2">
+      <c r="G213" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H213" t="s" s="2">
+      <c r="H213" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I213" t="s" s="2">
+      <c r="I213" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -6424,10 +6436,10 @@
       <c r="I218">
         <f>((C218-C217)^2+(D218- D217)^2)^.5</f>
       </c>
-      <c r="J218" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K218" s="2" t="s">
+      <c r="J218" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K218" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L218" t="n">
@@ -6471,28 +6483,28 @@
       </c>
     </row>
     <row r="220">
-      <c r="A220" t="s" s="2">
+      <c r="A220" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B220" t="s" s="2">
+      <c r="B220" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C220" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D220" t="s" s="2">
+      <c r="C220" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D220" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E220" t="s" s="2">
+      <c r="E220" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F220" t="s" s="2">
+      <c r="F220" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G220" t="s" s="2">
+      <c r="G220" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H220" t="s" s="2">
+      <c r="H220" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -6517,28 +6529,28 @@
       </c>
     </row>
     <row r="222">
-      <c r="B222" t="s" s="2">
+      <c r="B222" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C222" t="s" s="2">
+      <c r="C222" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D222" t="s" s="2">
+      <c r="D222" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E222" t="s" s="2">
+      <c r="E222" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F222" t="s" s="2">
+      <c r="F222" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G222" t="s" s="2">
+      <c r="G222" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H222" t="s" s="2">
+      <c r="H222" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I222" t="s" s="2">
+      <c r="I222" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -6597,10 +6609,10 @@
       <c r="I224">
         <f>((C224-C223)^2+(D224- D223)^2)^.5</f>
       </c>
-      <c r="J224" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K224" s="2" t="s">
+      <c r="J224" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K224" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L224" t="n">
@@ -6644,28 +6656,28 @@
       </c>
     </row>
     <row r="226">
-      <c r="A226" t="s" s="2">
+      <c r="A226" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B226" t="s" s="2">
+      <c r="B226" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C226" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D226" t="s" s="2">
+      <c r="C226" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D226" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E226" t="s" s="2">
+      <c r="E226" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F226" t="s" s="2">
+      <c r="F226" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G226" t="s" s="2">
+      <c r="G226" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H226" t="s" s="2">
+      <c r="H226" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -6690,28 +6702,28 @@
       </c>
     </row>
     <row r="228">
-      <c r="B228" t="s" s="2">
+      <c r="B228" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C228" t="s" s="2">
+      <c r="C228" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D228" t="s" s="2">
+      <c r="D228" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E228" t="s" s="2">
+      <c r="E228" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F228" t="s" s="2">
+      <c r="F228" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G228" t="s" s="2">
+      <c r="G228" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H228" t="s" s="2">
+      <c r="H228" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I228" t="s" s="2">
+      <c r="I228" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -6973,10 +6985,10 @@
       <c r="I237">
         <f>((C237-C236)^2+(D237- D236)^2)^.5</f>
       </c>
-      <c r="J237" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K237" s="2" t="s">
+      <c r="J237" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K237" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L237" t="n">
@@ -7020,28 +7032,28 @@
       </c>
     </row>
     <row r="239">
-      <c r="A239" t="s" s="2">
+      <c r="A239" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B239" t="s" s="2">
+      <c r="B239" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C239" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D239" t="s" s="2">
+      <c r="C239" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D239" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E239" t="s" s="2">
+      <c r="E239" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F239" t="s" s="2">
+      <c r="F239" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G239" t="s" s="2">
+      <c r="G239" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H239" t="s" s="2">
+      <c r="H239" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -7066,28 +7078,28 @@
       </c>
     </row>
     <row r="241">
-      <c r="B241" t="s" s="2">
+      <c r="B241" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C241" t="s" s="2">
+      <c r="C241" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D241" t="s" s="2">
+      <c r="D241" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E241" t="s" s="2">
+      <c r="E241" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F241" t="s" s="2">
+      <c r="F241" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G241" t="s" s="2">
+      <c r="G241" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H241" t="s" s="2">
+      <c r="H241" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I241" t="s" s="2">
+      <c r="I241" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -7146,10 +7158,10 @@
       <c r="I243">
         <f>((C243-C242)^2+(D243- D242)^2)^.5</f>
       </c>
-      <c r="J243" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K243" s="2" t="s">
+      <c r="J243" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K243" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L243" t="n">
@@ -7193,28 +7205,28 @@
       </c>
     </row>
     <row r="245">
-      <c r="A245" t="s" s="2">
+      <c r="A245" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B245" t="s" s="2">
+      <c r="B245" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C245" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D245" t="s" s="2">
+      <c r="C245" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D245" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E245" t="s" s="2">
+      <c r="E245" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F245" t="s" s="2">
+      <c r="F245" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G245" t="s" s="2">
+      <c r="G245" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H245" t="s" s="2">
+      <c r="H245" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -7239,28 +7251,28 @@
       </c>
     </row>
     <row r="247">
-      <c r="B247" t="s" s="2">
+      <c r="B247" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C247" t="s" s="2">
+      <c r="C247" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D247" t="s" s="2">
+      <c r="D247" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E247" t="s" s="2">
+      <c r="E247" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F247" t="s" s="2">
+      <c r="F247" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G247" t="s" s="2">
+      <c r="G247" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H247" t="s" s="2">
+      <c r="H247" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I247" t="s" s="2">
+      <c r="I247" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -7319,10 +7331,10 @@
       <c r="I249">
         <f>((C249-C248)^2+(D249- D248)^2)^.5</f>
       </c>
-      <c r="J249" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K249" s="2" t="s">
+      <c r="J249" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K249" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L249" t="n">
@@ -7366,28 +7378,28 @@
       </c>
     </row>
     <row r="251">
-      <c r="A251" t="s" s="2">
+      <c r="A251" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B251" t="s" s="2">
+      <c r="B251" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C251" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D251" t="s" s="2">
+      <c r="C251" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D251" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E251" t="s" s="2">
+      <c r="E251" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F251" t="s" s="2">
+      <c r="F251" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G251" t="s" s="2">
+      <c r="G251" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H251" t="s" s="2">
+      <c r="H251" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -7412,28 +7424,28 @@
       </c>
     </row>
     <row r="253">
-      <c r="B253" t="s" s="2">
+      <c r="B253" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C253" t="s" s="2">
+      <c r="C253" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D253" t="s" s="2">
+      <c r="D253" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E253" t="s" s="2">
+      <c r="E253" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F253" t="s" s="2">
+      <c r="F253" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G253" t="s" s="2">
+      <c r="G253" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H253" t="s" s="2">
+      <c r="H253" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I253" t="s" s="2">
+      <c r="I253" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -7550,10 +7562,10 @@
       <c r="I257">
         <f>((C257-C256)^2+(D257- D256)^2)^.5</f>
       </c>
-      <c r="J257" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K257" s="2" t="s">
+      <c r="J257" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K257" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L257" t="n">
@@ -7597,28 +7609,28 @@
       </c>
     </row>
     <row r="259">
-      <c r="A259" t="s" s="2">
+      <c r="A259" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B259" t="s" s="2">
+      <c r="B259" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C259" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D259" t="s" s="2">
+      <c r="C259" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D259" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E259" t="s" s="2">
+      <c r="E259" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F259" t="s" s="2">
+      <c r="F259" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G259" t="s" s="2">
+      <c r="G259" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H259" t="s" s="2">
+      <c r="H259" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -7643,28 +7655,28 @@
       </c>
     </row>
     <row r="261">
-      <c r="B261" t="s" s="2">
+      <c r="B261" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C261" t="s" s="2">
+      <c r="C261" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D261" t="s" s="2">
+      <c r="D261" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E261" t="s" s="2">
+      <c r="E261" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F261" t="s" s="2">
+      <c r="F261" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G261" t="s" s="2">
+      <c r="G261" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H261" t="s" s="2">
+      <c r="H261" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I261" t="s" s="2">
+      <c r="I261" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -7723,10 +7735,10 @@
       <c r="I263">
         <f>((C263-C262)^2+(D263- D262)^2)^.5</f>
       </c>
-      <c r="J263" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K263" s="2" t="s">
+      <c r="J263" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K263" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L263" t="n">
@@ -7770,28 +7782,28 @@
       </c>
     </row>
     <row r="265">
-      <c r="A265" t="s" s="2">
+      <c r="A265" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B265" t="s" s="2">
+      <c r="B265" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C265" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D265" t="s" s="2">
+      <c r="C265" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D265" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E265" t="s" s="2">
+      <c r="E265" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F265" t="s" s="2">
+      <c r="F265" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G265" t="s" s="2">
+      <c r="G265" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H265" t="s" s="2">
+      <c r="H265" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -7816,28 +7828,28 @@
       </c>
     </row>
     <row r="267">
-      <c r="B267" t="s" s="2">
+      <c r="B267" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C267" t="s" s="2">
+      <c r="C267" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D267" t="s" s="2">
+      <c r="D267" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E267" t="s" s="2">
+      <c r="E267" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F267" t="s" s="2">
+      <c r="F267" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G267" t="s" s="2">
+      <c r="G267" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H267" t="s" s="2">
+      <c r="H267" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I267" t="s" s="2">
+      <c r="I267" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -7896,10 +7908,10 @@
       <c r="I269">
         <f>((C269-C268)^2+(D269- D268)^2)^.5</f>
       </c>
-      <c r="J269" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K269" s="2" t="s">
+      <c r="J269" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K269" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L269" t="n">
@@ -7943,28 +7955,28 @@
       </c>
     </row>
     <row r="271">
-      <c r="A271" t="s" s="2">
+      <c r="A271" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B271" t="s" s="2">
+      <c r="B271" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C271" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D271" t="s" s="2">
+      <c r="C271" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D271" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E271" t="s" s="2">
+      <c r="E271" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F271" t="s" s="2">
+      <c r="F271" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G271" t="s" s="2">
+      <c r="G271" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H271" t="s" s="2">
+      <c r="H271" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -7989,28 +8001,28 @@
       </c>
     </row>
     <row r="273">
-      <c r="B273" t="s" s="2">
+      <c r="B273" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C273" t="s" s="2">
+      <c r="C273" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D273" t="s" s="2">
+      <c r="D273" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E273" t="s" s="2">
+      <c r="E273" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F273" t="s" s="2">
+      <c r="F273" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G273" t="s" s="2">
+      <c r="G273" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H273" t="s" s="2">
+      <c r="H273" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I273" t="s" s="2">
+      <c r="I273" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -8069,10 +8081,10 @@
       <c r="I275">
         <f>((C275-C274)^2+(D275- D274)^2)^.5</f>
       </c>
-      <c r="J275" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K275" s="2" t="s">
+      <c r="J275" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K275" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L275" t="n">
@@ -8116,28 +8128,28 @@
       </c>
     </row>
     <row r="277">
-      <c r="A277" t="s" s="2">
+      <c r="A277" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B277" t="s" s="2">
+      <c r="B277" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C277" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D277" t="s" s="2">
+      <c r="C277" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D277" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E277" t="s" s="2">
+      <c r="E277" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F277" t="s" s="2">
+      <c r="F277" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G277" t="s" s="2">
+      <c r="G277" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H277" t="s" s="2">
+      <c r="H277" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -8162,28 +8174,28 @@
       </c>
     </row>
     <row r="279">
-      <c r="B279" t="s" s="2">
+      <c r="B279" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C279" t="s" s="2">
+      <c r="C279" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D279" t="s" s="2">
+      <c r="D279" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E279" t="s" s="2">
+      <c r="E279" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F279" t="s" s="2">
+      <c r="F279" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G279" t="s" s="2">
+      <c r="G279" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H279" t="s" s="2">
+      <c r="H279" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I279" t="s" s="2">
+      <c r="I279" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -8242,10 +8254,10 @@
       <c r="I281">
         <f>((C281-C280)^2+(D281- D280)^2)^.5</f>
       </c>
-      <c r="J281" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K281" s="2" t="s">
+      <c r="J281" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K281" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L281" t="n">
@@ -8289,28 +8301,28 @@
       </c>
     </row>
     <row r="283">
-      <c r="A283" t="s" s="2">
+      <c r="A283" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B283" t="s" s="2">
+      <c r="B283" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C283" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D283" t="s" s="2">
+      <c r="C283" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D283" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E283" t="s" s="2">
+      <c r="E283" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F283" t="s" s="2">
+      <c r="F283" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G283" t="s" s="2">
+      <c r="G283" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H283" t="s" s="2">
+      <c r="H283" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -8335,28 +8347,28 @@
       </c>
     </row>
     <row r="285">
-      <c r="B285" t="s" s="2">
+      <c r="B285" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C285" t="s" s="2">
+      <c r="C285" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D285" t="s" s="2">
+      <c r="D285" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E285" t="s" s="2">
+      <c r="E285" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F285" t="s" s="2">
+      <c r="F285" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G285" t="s" s="2">
+      <c r="G285" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H285" t="s" s="2">
+      <c r="H285" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I285" t="s" s="2">
+      <c r="I285" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -8444,10 +8456,10 @@
       <c r="I288">
         <f>((C288-C287)^2+(D288- D287)^2)^.5</f>
       </c>
-      <c r="J288" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K288" s="2" t="s">
+      <c r="J288" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K288" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L288" t="n">
@@ -8491,28 +8503,28 @@
       </c>
     </row>
     <row r="290">
-      <c r="A290" t="s" s="2">
+      <c r="A290" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B290" t="s" s="2">
+      <c r="B290" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C290" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D290" t="s" s="2">
+      <c r="C290" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D290" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E290" t="s" s="2">
+      <c r="E290" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F290" t="s" s="2">
+      <c r="F290" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G290" t="s" s="2">
+      <c r="G290" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H290" t="s" s="2">
+      <c r="H290" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -8537,28 +8549,28 @@
       </c>
     </row>
     <row r="292">
-      <c r="B292" t="s" s="2">
+      <c r="B292" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C292" t="s" s="2">
+      <c r="C292" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D292" t="s" s="2">
+      <c r="D292" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E292" t="s" s="2">
+      <c r="E292" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F292" t="s" s="2">
+      <c r="F292" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G292" t="s" s="2">
+      <c r="G292" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H292" t="s" s="2">
+      <c r="H292" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I292" t="s" s="2">
+      <c r="I292" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -8646,10 +8658,10 @@
       <c r="I295">
         <f>((C295-C294)^2+(D295- D294)^2)^.5</f>
       </c>
-      <c r="J295" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K295" s="2" t="s">
+      <c r="J295" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K295" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L295" t="n">
@@ -8693,28 +8705,28 @@
       </c>
     </row>
     <row r="297">
-      <c r="A297" t="s" s="2">
+      <c r="A297" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B297" t="s" s="2">
+      <c r="B297" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C297" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D297" t="s" s="2">
+      <c r="C297" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="D297" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E297" t="s" s="2">
+      <c r="E297" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="F297" t="s" s="2">
+      <c r="F297" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="G297" t="s" s="2">
+      <c r="G297" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="H297" t="s" s="2">
+      <c r="H297" t="s" s="4">
         <v>16</v>
       </c>
     </row>
@@ -8739,28 +8751,28 @@
       </c>
     </row>
     <row r="299">
-      <c r="B299" t="s" s="2">
+      <c r="B299" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="C299" t="s" s="2">
+      <c r="C299" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D299" t="s" s="2">
+      <c r="D299" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E299" t="s" s="2">
+      <c r="E299" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F299" t="s" s="2">
+      <c r="F299" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G299" t="s" s="2">
+      <c r="G299" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H299" t="s" s="2">
+      <c r="H299" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I299" t="s" s="2">
+      <c r="I299" t="s" s="4">
         <v>11</v>
       </c>
     </row>
@@ -8819,10 +8831,10 @@
       <c r="I301">
         <f>((C301-C300)^2+(D301- D300)^2)^.5</f>
       </c>
-      <c r="J301" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K301" s="2" t="s">
+      <c r="J301" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K301" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L301" t="n">

</xml_diff>